<commit_message>
Working multicolumn. Broken import fixed
</commit_message>
<xml_diff>
--- a/Shiny App/data_files/Clean_Multi_Column.xlsx
+++ b/Shiny App/data_files/Clean_Multi_Column.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannehue\Desktop\Data_Visualization\Shiny App\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5473750-52AC-4761-91D9-8EA2311C0E40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E2304D-F70F-4ABE-BD23-650EE07DF702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39960" yWindow="2232" windowWidth="13980" windowHeight="12660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>